<commit_message>
19 avril, changements selon presentation
</commit_message>
<xml_diff>
--- a/PYTHON/xls dump/magic pie 1 datasheet.xlsx
+++ b/PYTHON/xls dump/magic pie 1 datasheet.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\libs\desktop\GitHub\electric-wheel-chair-trip-power-calculator\PYTHON\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\libraries\Desktop\GitHub\electric-wheel-chair-trip-power-calculator\PYTHON\xls dump\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="1"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="21570" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="magic pie 1 datasheet" sheetId="1" r:id="rId1"/>
     <sheet name="eff plot for 24v" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -9035,6 +9035,885 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-CA"/>
+              <a:t>Torque Curve 24 V</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.16719160104986883"/>
+                  <c:y val="-0.44775809273840772"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'magic pie 1 datasheet'!$B$310:$B$398</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="89"/>
+                <c:pt idx="0">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>177</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>177</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>177</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>163</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>130</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'magic pie 1 datasheet'!$A$310:$A$398</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="89"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.05</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.21</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.74</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.65</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.86</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.12</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.2200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.38</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.61</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.88</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.98</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.18</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.45</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.58</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.74</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.04</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.41</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.3499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.6500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.08</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.27</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.37</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.74</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6.07</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6.36</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>6.61</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>6.87</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>7.31</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7.33</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>7.66</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>8.1199999999999992</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>8.14</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>8.59</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>8.94</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>9.16</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>9.56</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>9.9600000000000009</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>10.039999999999999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>10.43</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>10.58</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>10.99</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>11.46</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>11.56</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>12.13</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>12.7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>13.29</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>13.4</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>13.89</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>13.95</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>14.29</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>14.63</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>15.1</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>15.15</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>15.42</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>15.82</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>16.12</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>16.46</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>16.78</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>17.32</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>17.37</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>17.64</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>18.02</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>18.34</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>18.899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>19.29</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>19.88</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>20.05</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>20.48</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>20.6</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>21.02</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>21.3</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>21.75</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>22.01</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>22.43</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>22.63</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E63B-41F5-8FB1-C6EDC6E5FD5B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="510828144"/>
+        <c:axId val="510833064"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="510828144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="510833064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="510833064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="510828144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9820,6 +10699,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -13433,6 +14352,522 @@
 </file>
 
 <file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -14209,6 +15644,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>414618</xdr:colOff>
+      <xdr:row>305</xdr:row>
+      <xdr:rowOff>96371</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>56029</xdr:colOff>
+      <xdr:row>322</xdr:row>
+      <xdr:rowOff>123265</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24B29A30-70C4-4806-B2A1-F0ECB70FE266}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -14557,8 +16028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q410"/>
   <sheetViews>
-    <sheetView topLeftCell="B283" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G356" sqref="B285:G356"/>
+    <sheetView tabSelected="1" topLeftCell="C302" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M306" sqref="M306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23322,7 +24793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B2" sqref="A2:B36"/>
     </sheetView>
   </sheetViews>

</xml_diff>